<commit_message>
Adding SVs to reduced model
</commit_message>
<xml_diff>
--- a/metadata/4_GSE156101.xlsx
+++ b/metadata/4_GSE156101.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shdam/Dropbox/05_1_individual_study_excel_KVS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/sohdam_dtu_dk/Documents/Rprojects/pairedGSEA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0AFAB9-943D-7445-8D51-526CCC445594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9D0AFAB9-943D-7445-8D51-526CCC445594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9ABC88E-7CB3-324D-B3E0-7A03E14A6CAE}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="27980" windowHeight="11000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>TP53 Knockout</t>
   </si>
   <si>
-    <t>TP53 and TNKS1/2T Knockout</t>
-  </si>
-  <si>
     <t>2v3</t>
   </si>
   <si>
@@ -122,6 +119,9 @@
   </si>
   <si>
     <t>3v4</t>
+  </si>
+  <si>
+    <t>TP53 and TNKS1-2T Knockout</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -602,7 +602,7 @@
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -622,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -642,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -662,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>